<commit_message>
5/4 Work and added Thread IDs
</commit_message>
<xml_diff>
--- a/Tracing.xlsx
+++ b/Tracing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>I</t>
   </si>
@@ -72,25 +72,22 @@
     <t>G-G</t>
   </si>
   <si>
-    <t>9-12</t>
-  </si>
-  <si>
-    <t>10-13</t>
-  </si>
-  <si>
-    <t>16-19</t>
-  </si>
-  <si>
-    <t>22-25</t>
-  </si>
-  <si>
-    <t>6-9</t>
-  </si>
-  <si>
     <t>13-16</t>
   </si>
   <si>
-    <t>19-22</t>
+    <t>7-10</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>8-11</t>
+  </si>
+  <si>
+    <t>14-18</t>
+  </si>
+  <si>
+    <t>1-4</t>
   </si>
 </sst>
 </file>
@@ -111,7 +108,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,30 +119,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor rgb="FF0000FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -206,30 +179,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -596,7 +564,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -619,13 +587,13 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1"/>
@@ -635,13 +603,13 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1"/>
@@ -651,13 +619,13 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1"/>
@@ -667,13 +635,13 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="1"/>
@@ -683,13 +651,13 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="1"/>
@@ -710,89 +678,81 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>20</v>
+      <c r="D10" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="10">
-        <v>30</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>23</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="10"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>

</xml_diff>